<commit_message>
Everything is done at 1
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
+++ b/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="41">
   <si>
     <t>User Name</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>P</t>
-  </si>
-  <si>
-    <t>P**</t>
   </si>
   <si>
     <t>U</t>
@@ -596,13 +593,13 @@
         <v>25</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s" s="0">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="P6" t="s" s="0">
         <v>25</v>
@@ -634,40 +631,40 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="L7" t="s" s="0">
-        <v>35</v>
       </c>
       <c r="M7" t="s" s="0">
         <v>25</v>
@@ -708,7 +705,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>25</v>
@@ -759,7 +756,7 @@
         <v>25</v>
       </c>
       <c r="R8" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S8" t="s" s="0">
         <v>25</v>
@@ -782,7 +779,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>25</v>
@@ -818,10 +815,10 @@
         <v>25</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O9" t="s" s="0">
         <v>25</v>
@@ -856,7 +853,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>25</v>
@@ -930,7 +927,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>25</v>
@@ -1004,10 +1001,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>25</v>
@@ -1019,7 +1016,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s" s="0">
         <v>28</v>
@@ -1034,7 +1031,7 @@
         <v>25</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L12" t="s" s="0">
         <v>25</v>
@@ -1043,7 +1040,7 @@
         <v>28</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O12" t="s" s="0">
         <v>25</v>
@@ -1067,7 +1064,7 @@
         <v>25</v>
       </c>
       <c r="V12" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W12" t="s" s="0">
         <v>31</v>

</xml_diff>

<commit_message>
Changes made in searchByMonth
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
+++ b/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="42">
   <si>
     <t>User Name</t>
   </si>
@@ -92,37 +92,40 @@
     <t/>
   </si>
   <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>Amit Patel</t>
   </si>
   <si>
     <t>Anjali Desai</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Pooja Mehta</t>
   </si>
   <si>
     <t>R Rohit</t>
   </si>
   <si>
-    <t>P</t>
+    <t>Tejaswini</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Pradeep</t>
+  </si>
+  <si>
+    <t>Rajeev</t>
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>Tejaswini</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Pradeep</t>
-  </si>
-  <si>
-    <t>Rajeev</t>
   </si>
   <si>
     <t>Neha Gupta</t>
@@ -179,7 +182,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -341,7 +344,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>25</v>
@@ -377,7 +380,7 @@
         <v>25</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s" s="0">
         <v>25</v>
@@ -409,7 +412,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>25</v>
@@ -451,7 +454,7 @@
         <v>25</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s" s="0">
         <v>25</v>
@@ -483,7 +486,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>25</v>
@@ -525,7 +528,7 @@
         <v>25</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P5" t="s" s="0">
         <v>25</v>
@@ -552,95 +555,95 @@
         <v>25</v>
       </c>
       <c r="X5" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>25</v>
       </c>
       <c r="C6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="U6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="V6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="W6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="X6" t="s" s="0">
         <v>28</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="P6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="Q6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="R6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="S6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="T6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="U6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="V6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="W6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="X6" t="s" s="0">
-        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>25</v>
@@ -649,46 +652,46 @@
         <v>25</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="M7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="Q7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="S7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U7" t="s" s="0">
         <v>25</v>
@@ -705,7 +708,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>25</v>
@@ -738,7 +741,7 @@
         <v>25</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s" s="0">
         <v>25</v>
@@ -756,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="R8" t="s" s="0">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="S8" t="s" s="0">
         <v>25</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>25</v>
@@ -818,7 +821,7 @@
         <v>25</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="O9" t="s" s="0">
         <v>25</v>
@@ -830,7 +833,7 @@
         <v>25</v>
       </c>
       <c r="R9" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="S9" t="s" s="0">
         <v>25</v>
@@ -853,46 +856,46 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="M10" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="J10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="K10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="L10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="M10" t="s" s="0">
-        <v>25</v>
-      </c>
       <c r="N10" t="s" s="0">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="O10" t="s" s="0">
         <v>25</v>
@@ -939,7 +942,7 @@
         <v>25</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>25</v>
@@ -1004,72 +1007,146 @@
         <v>39</v>
       </c>
       <c r="B12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="M12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="S12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="T12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="U12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="V12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="W12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="X12" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s" s="0">
+      <c r="C13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="H12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="J12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="K12" t="s" s="0">
+      <c r="H13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="L12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="M12" t="s" s="0">
+      <c r="L13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="N12" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="O12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="P12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="Q12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="R12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="S12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="T12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="U12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="V12" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="W12" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="X12" t="s" s="0">
+      <c r="N13" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="S13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="T13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="U13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="V13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="W13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="X13" t="s" s="0">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes in login , create , update
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
+++ b/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="41">
   <si>
     <t>User Name</t>
   </si>
@@ -92,25 +92,25 @@
     <t/>
   </si>
   <si>
-    <t>Sneha</t>
+    <t>Amit Patel</t>
+  </si>
+  <si>
+    <t>Anjali Desai</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Pooja Mehta</t>
+  </si>
+  <si>
+    <t>R Rohit</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Amit Patel</t>
-  </si>
-  <si>
-    <t>Anjali Desai</t>
-  </si>
-  <si>
-    <t>Pooja Mehta</t>
-  </si>
-  <si>
-    <t>R Rohit</t>
+    <t>U</t>
   </si>
   <si>
     <t>Tejaswini</t>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Rajeev</t>
-  </si>
-  <si>
-    <t>U</t>
   </si>
   <si>
     <t>Neha Gupta</t>
@@ -182,7 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -344,7 +341,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>25</v>
@@ -380,7 +377,7 @@
         <v>25</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s" s="0">
         <v>25</v>
@@ -412,7 +409,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>25</v>
@@ -454,7 +451,7 @@
         <v>25</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s" s="0">
         <v>25</v>
@@ -486,7 +483,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>25</v>
@@ -528,66 +525,66 @@
         <v>25</v>
       </c>
       <c r="O5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="S5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="U5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="V5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="W5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="X5" t="s" s="0">
         <v>28</v>
-      </c>
-      <c r="P5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="Q5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="R5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="S5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="T5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="U5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="V5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="W5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="X5" t="s" s="0">
-        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>25</v>
-      </c>
       <c r="H6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>25</v>
@@ -596,10 +593,10 @@
         <v>25</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s" s="0">
         <v>25</v>
@@ -608,16 +605,16 @@
         <v>25</v>
       </c>
       <c r="Q6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="R6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="S6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="T6" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="U6" t="s" s="0">
         <v>25</v>
@@ -629,21 +626,21 @@
         <v>25</v>
       </c>
       <c r="X6" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>25</v>
@@ -652,46 +649,46 @@
         <v>25</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="Q7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T7" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U7" t="s" s="0">
         <v>25</v>
@@ -708,7 +705,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>25</v>
@@ -741,25 +738,25 @@
         <v>25</v>
       </c>
       <c r="L8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R8" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="M8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="N8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="O8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="P8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="Q8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="R8" t="s" s="0">
-        <v>25</v>
       </c>
       <c r="S8" t="s" s="0">
         <v>25</v>
@@ -782,7 +779,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>25</v>
@@ -821,7 +818,7 @@
         <v>25</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="O9" t="s" s="0">
         <v>25</v>
@@ -833,7 +830,7 @@
         <v>25</v>
       </c>
       <c r="R9" t="s" s="0">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="S9" t="s" s="0">
         <v>25</v>
@@ -856,7 +853,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>25</v>
@@ -892,10 +889,10 @@
         <v>25</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="O10" t="s" s="0">
         <v>25</v>
@@ -942,7 +939,7 @@
         <v>25</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>25</v>
@@ -1007,7 +1004,7 @@
         <v>39</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>25</v>
@@ -1016,14 +1013,14 @@
         <v>25</v>
       </c>
       <c r="E12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>25</v>
-      </c>
       <c r="H12" t="s" s="0">
         <v>25</v>
       </c>
@@ -1034,16 +1031,16 @@
         <v>25</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="L12" t="s" s="0">
         <v>25</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O12" t="s" s="0">
         <v>25</v>
@@ -1067,86 +1064,12 @@
         <v>25</v>
       </c>
       <c r="V12" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="W12" t="s" s="0">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="X12" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="G13" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="J13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="K13" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="L13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="M13" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="N13" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="O13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="P13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="Q13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="R13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="S13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="T13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="U13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="V13" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="W13" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="X13" t="s" s="0">
         <v>25</v>
       </c>
     </row>

</xml_diff>